<commit_message>
Correlaciones en SubSaturado y Saturado
</commit_message>
<xml_diff>
--- a/files/reservorio_empuje_gas.xlsx
+++ b/files/reservorio_empuje_gas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\Desktop\py\ayllin\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC620195-6475-44F9-B41C-6C987D312844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8954E00B-06CC-4BA1-8841-E2647E1D8020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3930" windowWidth="14415" windowHeight="11550" xr2:uid="{44499CD8-C7FF-4958-889A-4A80EC9AE5DF}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:G12"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +446,7 @@
         <v>1.6291</v>
       </c>
       <c r="E2">
-        <v>4.32355</v>
+        <v>4.3235499999999998E-3</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -464,7 +464,7 @@
         <v>1.6839</v>
       </c>
       <c r="E3">
-        <v>4.4358500000000003</v>
+        <v>4.4358499999999999E-3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -481,7 +481,7 @@
         <v>1.7835000000000001</v>
       </c>
       <c r="E4">
-        <v>4.8850499999999997</v>
+        <v>4.8850500000000002E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -498,7 +498,7 @@
         <v>1.911</v>
       </c>
       <c r="E5">
-        <v>5.5588499999999996</v>
+        <v>5.5588499999999997E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SubSaturado - Beggs con problemas
</commit_message>
<xml_diff>
--- a/files/reservorio_empuje_gas.xlsx
+++ b/files/reservorio_empuje_gas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\Desktop\py\ayllin\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8954E00B-06CC-4BA1-8841-E2647E1D8020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D034B5-06F2-4AB3-BF39-049BB23C5C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3930" windowWidth="14415" windowHeight="11550" xr2:uid="{44499CD8-C7FF-4958-889A-4A80EC9AE5DF}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>p</t>
-  </si>
-  <si>
     <t>Np</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>Bg</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -415,26 +415,26 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>